<commit_message>
app inin process done
</commit_message>
<xml_diff>
--- a/db/doc/IndividualStockAcount.xlsx
+++ b/db/doc/IndividualStockAcount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiho/Desktop/DB_API_assignment/db/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70397C89-EA57-D849-91AB-332D41CFD40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C31C1BD-8B5C-3240-A3A2-E12451ABEDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34140" yWindow="500" windowWidth="17060" windowHeight="27040" xr2:uid="{0F52580C-D0CC-404F-9E7A-49470998494F}"/>
+    <workbookView xWindow="24740" yWindow="500" windowWidth="25600" windowHeight="27040" xr2:uid="{0F52580C-D0CC-404F-9E7A-49470998494F}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualStockAcount" sheetId="2" r:id="rId1"/>
@@ -36,16 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
-  <si>
-    <t>jiho266</t>
-  </si>
-  <si>
-    <t>jiho267</t>
-  </si>
-  <si>
-    <t>jiho268</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -62,25 +53,34 @@
     <t>005930</t>
   </si>
   <si>
-    <t>삼성전자</t>
-  </si>
-  <si>
     <t>035420</t>
   </si>
   <si>
-    <t>NAVER</t>
-  </si>
-  <si>
     <t>000660</t>
   </si>
   <si>
-    <t>SK하이닉스</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>jiho270</t>
+    <t>user270</t>
+  </si>
+  <si>
+    <t>hoho222</t>
+  </si>
+  <si>
+    <t>nick0422</t>
+  </si>
+  <si>
+    <t>jiho264</t>
+  </si>
+  <si>
+    <t>hseop884</t>
+  </si>
+  <si>
+    <t>086520</t>
+  </si>
+  <si>
+    <t>247540</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,30 +453,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -487,13 +484,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -504,13 +498,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -521,13 +512,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -538,13 +526,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -555,13 +540,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -572,13 +554,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -588,10 +567,32 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="2"/>
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="2"/>
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>

</xml_diff>

<commit_message>
circle plot bug fix, add nps stock acount
</commit_message>
<xml_diff>
--- a/db/doc/IndividualStockAcount.xlsx
+++ b/db/doc/IndividualStockAcount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiho/Desktop/DB_API_assignment/db/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C31C1BD-8B5C-3240-A3A2-E12451ABEDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF21ABC7-EB29-914E-AC3F-2B7BFBFEF508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24740" yWindow="500" windowWidth="25600" windowHeight="27040" xr2:uid="{0F52580C-D0CC-404F-9E7A-49470998494F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>247540</t>
+  </si>
+  <si>
+    <t>009150</t>
+  </si>
+  <si>
+    <t>336370</t>
   </si>
 </sst>
 </file>
@@ -443,7 +449,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,10 +601,32 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>

</xml_diff>